<commit_message>
Add missing Irgason variables for Bernard spruce most East
</commit_message>
<xml_diff>
--- a/Resources/Variable_description_full.xlsx
+++ b/Resources/Variable_description_full.xlsx
@@ -1,11 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="158" documentId="13_ncr:1_{D9D14E5E-F476-45BE-9422-600D3D140919}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{84578043-0930-4EAA-9677-BFF991232646}"/>
+  <xr:revisionPtr revIDLastSave="162" documentId="13_ncr:1_{D9D14E5E-F476-45BE-9422-600D3D140919}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3078C1A2-814B-46D3-B6F9-0FC82E8013FB}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="819" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="819" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="6" xr2:uid="{FA0D2C8C-B83F-42B3-AEE0-8A421FCD5665}"/>
   </bookViews>
   <sheets>
     <sheet name="Bernard_lake_cs" sheetId="14" r:id="rId1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7690" uniqueCount="1227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7708" uniqueCount="1226">
   <si>
     <t>LI-7700</t>
   </si>
@@ -3330,9 +3331,6 @@
   </si>
   <si>
     <t>LI-7500</t>
-  </si>
-  <si>
-    <t>air_press_LI7500</t>
   </si>
   <si>
     <t>air_press_CS106</t>
@@ -4140,6 +4138,7 @@
     <sheetView topLeftCell="C27" workbookViewId="0">
       <selection activeCell="D39" sqref="D39"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -4669,10 +4668,10 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="B38" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="C38" t="s">
         <v>217</v>
@@ -4681,7 +4680,7 @@
         <v>81</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="F38" t="s">
         <v>223</v>
@@ -4709,10 +4708,10 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B40" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="C40" t="s">
         <v>457</v>
@@ -4721,7 +4720,7 @@
         <v>2</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="F40" t="s">
         <v>462</v>
@@ -4769,10 +4768,10 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="B43" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="C43" t="s">
         <v>208</v>
@@ -4781,7 +4780,7 @@
         <v>142</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="F43" t="s">
         <v>461</v>
@@ -4849,10 +4848,10 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="B47" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="C47" t="s">
         <v>458</v>
@@ -4861,7 +4860,7 @@
         <v>142</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="F47" t="s">
         <v>461</v>
@@ -4869,10 +4868,10 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="B48" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="C48" t="s">
         <v>459</v>
@@ -4881,7 +4880,7 @@
         <v>142</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="F48" t="s">
         <v>461</v>
@@ -5483,7 +5482,7 @@
         <v>534</v>
       </c>
       <c r="E78" s="9" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="F78" t="s">
         <v>537</v>
@@ -5503,7 +5502,7 @@
         <v>534</v>
       </c>
       <c r="E79" s="9" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="F79" t="s">
         <v>537</v>
@@ -5523,7 +5522,7 @@
         <v>5</v>
       </c>
       <c r="E80" s="9" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="F80" t="s">
         <v>537</v>
@@ -5531,7 +5530,7 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="B81" t="s">
         <v>334</v>
@@ -7574,6 +7573,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -7606,7 +7606,7 @@
         <v>168</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>169</v>
@@ -8247,30 +8247,30 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
+        <v>1200</v>
+      </c>
+      <c r="B51" t="s">
+        <v>1206</v>
+      </c>
+      <c r="C51" t="s">
         <v>1201</v>
       </c>
-      <c r="B51" t="s">
-        <v>1207</v>
-      </c>
-      <c r="C51" t="s">
-        <v>1202</v>
-      </c>
       <c r="D51" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
+        <v>1202</v>
+      </c>
+      <c r="B52" t="s">
+        <v>1207</v>
+      </c>
+      <c r="C52" t="s">
         <v>1203</v>
       </c>
-      <c r="B52" t="s">
-        <v>1208</v>
-      </c>
-      <c r="C52" t="s">
-        <v>1204</v>
-      </c>
       <c r="D52" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
@@ -8443,13 +8443,13 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="B65" t="s">
         <v>809</v>
       </c>
       <c r="C65" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="D65" t="s">
         <v>736</v>
@@ -8457,13 +8457,13 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="B66" t="s">
         <v>810</v>
       </c>
       <c r="C66" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="D66" t="s">
         <v>736</v>
@@ -8471,13 +8471,13 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="B67" t="s">
         <v>811</v>
       </c>
       <c r="C67" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="D67" t="s">
         <v>736</v>
@@ -9641,6 +9641,7 @@
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -9753,7 +9754,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="B11" t="s">
         <v>115</v>
@@ -9797,7 +9798,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="B13" t="s">
         <v>133</v>
@@ -9818,7 +9819,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="B14" t="s">
         <v>134</v>
@@ -9839,7 +9840,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="B15" t="s">
         <v>137</v>
@@ -9860,7 +9861,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="B16" t="s">
         <v>138</v>
@@ -9881,7 +9882,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="B17" t="s">
         <v>135</v>
@@ -9901,7 +9902,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="B18" t="s">
         <v>136</v>
@@ -9921,7 +9922,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="B19" t="s">
         <v>141</v>
@@ -9941,7 +9942,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="B20" t="s">
         <v>128</v>
@@ -9961,7 +9962,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="B21" t="s">
         <v>131</v>
@@ -9981,7 +9982,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="B22" t="s">
         <v>132</v>
@@ -10184,6 +10185,7 @@
   <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -10371,7 +10373,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="B14" t="s">
         <v>1003</v>
@@ -10434,7 +10436,7 @@
         <v>917</v>
       </c>
       <c r="B17" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="C17" t="s">
         <v>516</v>
@@ -10454,7 +10456,7 @@
         <v>918</v>
       </c>
       <c r="B18" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="C18" t="s">
         <v>517</v>
@@ -10882,6 +10884,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -11005,6 +11008,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -11074,6 +11078,7 @@
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -11103,7 +11108,7 @@
         <v>168</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>169</v>
@@ -11880,44 +11885,44 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
+        <v>1197</v>
+      </c>
+      <c r="B60" t="s">
+        <v>1205</v>
+      </c>
+      <c r="C60" t="s">
         <v>1198</v>
       </c>
-      <c r="B60" t="s">
-        <v>1206</v>
-      </c>
-      <c r="C60" t="s">
+      <c r="D60" t="s">
         <v>1199</v>
-      </c>
-      <c r="D60" t="s">
-        <v>1200</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
+        <v>1200</v>
+      </c>
+      <c r="B61" t="s">
+        <v>1206</v>
+      </c>
+      <c r="C61" t="s">
         <v>1201</v>
       </c>
-      <c r="B61" t="s">
-        <v>1207</v>
-      </c>
-      <c r="C61" t="s">
-        <v>1202</v>
-      </c>
       <c r="D61" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
+        <v>1202</v>
+      </c>
+      <c r="B62" t="s">
+        <v>1207</v>
+      </c>
+      <c r="C62" t="s">
         <v>1203</v>
       </c>
-      <c r="B62" t="s">
-        <v>1208</v>
-      </c>
-      <c r="C62" t="s">
-        <v>1204</v>
-      </c>
       <c r="D62" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
@@ -12090,13 +12095,13 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="B75" t="s">
         <v>809</v>
       </c>
       <c r="C75" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="D75" t="s">
         <v>736</v>
@@ -12104,13 +12109,13 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="B76" t="s">
         <v>810</v>
       </c>
       <c r="C76" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="D76" t="s">
         <v>736</v>
@@ -12118,13 +12123,13 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="B77" t="s">
         <v>811</v>
       </c>
       <c r="C77" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="D77" t="s">
         <v>736</v>
@@ -13497,9 +13502,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A58" sqref="A58"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -14826,7 +14832,7 @@
         <v>534</v>
       </c>
       <c r="E77" s="9" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="F77" t="s">
         <v>537</v>
@@ -14846,7 +14852,7 @@
         <v>534</v>
       </c>
       <c r="E78" s="9" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="F78" t="s">
         <v>537</v>
@@ -14866,7 +14872,7 @@
         <v>5</v>
       </c>
       <c r="E79" s="9" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="F79" t="s">
         <v>537</v>
@@ -14874,7 +14880,7 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="B80" t="s">
         <v>334</v>
@@ -16919,8 +16925,9 @@
   <dimension ref="A1:E186"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A71" sqref="A71"/>
+      <selection activeCell="A58" sqref="A58"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -16950,7 +16957,7 @@
         <v>168</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>169</v>
@@ -17727,44 +17734,44 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
+        <v>1197</v>
+      </c>
+      <c r="B60" t="s">
+        <v>1205</v>
+      </c>
+      <c r="C60" t="s">
         <v>1198</v>
       </c>
-      <c r="B60" t="s">
-        <v>1206</v>
-      </c>
-      <c r="C60" t="s">
+      <c r="D60" t="s">
         <v>1199</v>
-      </c>
-      <c r="D60" t="s">
-        <v>1200</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
+        <v>1200</v>
+      </c>
+      <c r="B61" t="s">
+        <v>1206</v>
+      </c>
+      <c r="C61" t="s">
         <v>1201</v>
       </c>
-      <c r="B61" t="s">
-        <v>1207</v>
-      </c>
-      <c r="C61" t="s">
-        <v>1202</v>
-      </c>
       <c r="D61" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
+        <v>1202</v>
+      </c>
+      <c r="B62" t="s">
+        <v>1207</v>
+      </c>
+      <c r="C62" t="s">
         <v>1203</v>
       </c>
-      <c r="B62" t="s">
-        <v>1208</v>
-      </c>
-      <c r="C62" t="s">
-        <v>1204</v>
-      </c>
       <c r="D62" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
@@ -17937,13 +17944,13 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="B75" t="s">
         <v>809</v>
       </c>
       <c r="C75" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="D75" t="s">
         <v>736</v>
@@ -17951,13 +17958,13 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="B76" t="s">
         <v>810</v>
       </c>
       <c r="C76" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="D76" t="s">
         <v>736</v>
@@ -17965,13 +17972,13 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="B77" t="s">
         <v>811</v>
       </c>
       <c r="C77" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="D77" t="s">
         <v>736</v>
@@ -19347,6 +19354,7 @@
     <sheetView topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B67" sqref="B67"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -19821,7 +19829,7 @@
         <v>634</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>34</v>
@@ -19841,7 +19849,7 @@
         <v>635</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>34</v>
@@ -19861,7 +19869,7 @@
         <v>636</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>34</v>
@@ -19881,7 +19889,7 @@
         <v>30</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>34</v>
@@ -19901,7 +19909,7 @@
         <v>31</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>34</v>
@@ -19921,7 +19929,7 @@
         <v>32</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>34</v>
@@ -20320,7 +20328,7 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="B58" t="s">
         <v>13</v>
@@ -20341,7 +20349,7 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="B59" t="s">
         <v>78</v>
@@ -21827,6 +21835,7 @@
   <dimension ref="A1:E158"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -21859,7 +21868,7 @@
         <v>168</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>169</v>
@@ -22498,30 +22507,30 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
+        <v>1200</v>
+      </c>
+      <c r="B51" t="s">
+        <v>1206</v>
+      </c>
+      <c r="C51" t="s">
         <v>1201</v>
       </c>
-      <c r="B51" t="s">
-        <v>1207</v>
-      </c>
-      <c r="C51" t="s">
-        <v>1202</v>
-      </c>
       <c r="D51" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
+        <v>1202</v>
+      </c>
+      <c r="B52" t="s">
+        <v>1207</v>
+      </c>
+      <c r="C52" t="s">
         <v>1203</v>
       </c>
-      <c r="B52" t="s">
-        <v>1208</v>
-      </c>
-      <c r="C52" t="s">
-        <v>1204</v>
-      </c>
       <c r="D52" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
@@ -22694,13 +22703,13 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="B65" t="s">
         <v>809</v>
       </c>
       <c r="C65" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="D65" t="s">
         <v>736</v>
@@ -22708,13 +22717,13 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="B66" t="s">
         <v>810</v>
       </c>
       <c r="C66" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="D66" t="s">
         <v>736</v>
@@ -22722,13 +22731,13 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="B67" t="s">
         <v>811</v>
       </c>
       <c r="C67" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="D67" t="s">
         <v>736</v>
@@ -23888,8 +23897,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G152"/>
   <sheetViews>
-    <sheetView topLeftCell="C30" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
+    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="1">
+      <selection activeCell="A70" sqref="A70:XFD80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -24160,7 +24172,7 @@
         <v>1092</v>
       </c>
       <c r="C18" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="D18" t="s">
         <v>203</v>
@@ -24320,7 +24332,7 @@
         <v>916</v>
       </c>
       <c r="B33" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="C33" t="s">
         <v>515</v>
@@ -24357,10 +24369,10 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
+        <v>1099</v>
+      </c>
+      <c r="B35" t="s">
         <v>1100</v>
-      </c>
-      <c r="B35" t="s">
-        <v>1101</v>
       </c>
       <c r="C35" t="s">
         <v>217</v>
@@ -24369,7 +24381,7 @@
         <v>19</v>
       </c>
       <c r="E35" s="9" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="F35" t="s">
         <v>223</v>
@@ -24520,7 +24532,7 @@
         <v>407</v>
       </c>
       <c r="B43" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="C43" t="s">
         <v>541</v>
@@ -24840,7 +24852,7 @@
         <v>410</v>
       </c>
       <c r="B59" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="C59" t="s">
         <v>415</v>
@@ -24860,7 +24872,7 @@
         <v>412</v>
       </c>
       <c r="B60" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="C60" t="s">
         <v>417</v>
@@ -24880,7 +24892,7 @@
         <v>413</v>
       </c>
       <c r="B61" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="C61" t="s">
         <v>421</v>
@@ -24900,7 +24912,7 @@
         <v>433</v>
       </c>
       <c r="B62" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="C62" t="s">
         <v>431</v>
@@ -24920,7 +24932,7 @@
         <v>414</v>
       </c>
       <c r="B63" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="C63" t="s">
         <v>422</v>
@@ -24940,7 +24952,7 @@
         <v>434</v>
       </c>
       <c r="B64" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="C64" t="s">
         <v>432</v>
@@ -24960,7 +24972,7 @@
         <v>933</v>
       </c>
       <c r="B65" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="C65" t="s">
         <v>496</v>
@@ -24980,7 +24992,7 @@
         <v>929</v>
       </c>
       <c r="B66" s="13" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="C66" s="14" t="s">
         <v>447</v>
@@ -25001,7 +25013,7 @@
         <v>445</v>
       </c>
       <c r="B67" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="C67" t="s">
         <v>437</v>
@@ -25021,7 +25033,7 @@
         <v>444</v>
       </c>
       <c r="B68" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="C68" t="s">
         <v>438</v>
@@ -25041,7 +25053,7 @@
         <v>930</v>
       </c>
       <c r="B69" s="16" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="C69" s="16" t="s">
         <v>932</v>
@@ -25281,85 +25293,85 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A81" s="16" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="B81" s="16" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="C81" s="16" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="D81" s="16" t="s">
         <v>364</v>
       </c>
       <c r="E81" s="17" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="F81" s="16" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="G81" s="16"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A82" s="16" t="s">
+        <v>1180</v>
+      </c>
+      <c r="B82" s="16" t="s">
+        <v>1214</v>
+      </c>
+      <c r="C82" s="16" t="s">
+        <v>1182</v>
+      </c>
+      <c r="D82" s="16" t="s">
         <v>1181</v>
       </c>
-      <c r="B82" s="16" t="s">
-        <v>1215</v>
-      </c>
-      <c r="C82" s="16" t="s">
-        <v>1183</v>
-      </c>
-      <c r="D82" s="16" t="s">
-        <v>1182</v>
-      </c>
       <c r="E82" s="17" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="F82" s="16" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="G82" s="16"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A83" s="16" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="B83" s="16" t="s">
+        <v>1184</v>
+      </c>
+      <c r="C83" s="16" t="s">
         <v>1185</v>
-      </c>
-      <c r="C83" s="16" t="s">
-        <v>1186</v>
       </c>
       <c r="D83" s="16" t="s">
         <v>203</v>
       </c>
       <c r="E83" s="17" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="F83" s="16" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="G83" s="16"/>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A84" s="16" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="B84" s="16" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="C84" s="16" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="D84" s="16" t="s">
         <v>203</v>
       </c>
       <c r="E84" s="17" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="F84" s="16" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="G84" s="16"/>
     </row>
@@ -25465,25 +25477,25 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
+        <v>1173</v>
+      </c>
+      <c r="B90" t="s">
+        <v>1172</v>
+      </c>
+      <c r="C90" t="s">
         <v>1174</v>
-      </c>
-      <c r="B90" t="s">
-        <v>1173</v>
-      </c>
-      <c r="C90" t="s">
-        <v>1175</v>
       </c>
       <c r="D90" t="s">
         <v>203</v>
       </c>
       <c r="E90" s="9" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="F90" t="s">
+        <v>1175</v>
+      </c>
+      <c r="G90" t="s">
         <v>1176</v>
-      </c>
-      <c r="G90" t="s">
-        <v>1177</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.35">
@@ -25500,7 +25512,7 @@
         <v>534</v>
       </c>
       <c r="E91" s="9" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="F91" t="s">
         <v>537</v>
@@ -25540,7 +25552,7 @@
         <v>534</v>
       </c>
       <c r="E93" s="9" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="F93" t="s">
         <v>537</v>
@@ -25580,7 +25592,7 @@
         <v>5</v>
       </c>
       <c r="E95" s="9" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="F95" t="s">
         <v>537</v>
@@ -25648,7 +25660,7 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="B99" t="s">
         <v>334</v>
@@ -25671,7 +25683,7 @@
         <v>14</v>
       </c>
       <c r="B100" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="C100" t="s">
         <v>429</v>
@@ -25720,7 +25732,7 @@
         <v>203</v>
       </c>
       <c r="E102" s="9" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="F102" t="s">
         <v>188</v>
@@ -25751,7 +25763,7 @@
         <v>226</v>
       </c>
       <c r="B104" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="C104" t="s">
         <v>418</v>
@@ -25771,7 +25783,7 @@
         <v>226</v>
       </c>
       <c r="B105" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="C105" t="s">
         <v>419</v>
@@ -25791,7 +25803,7 @@
         <v>226</v>
       </c>
       <c r="B106" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="C106" t="s">
         <v>420</v>
@@ -25811,7 +25823,7 @@
         <v>226</v>
       </c>
       <c r="B107" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="C107" t="s">
         <v>439</v>
@@ -25831,7 +25843,7 @@
         <v>226</v>
       </c>
       <c r="B108" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="C108" t="s">
         <v>440</v>
@@ -25851,7 +25863,7 @@
         <v>226</v>
       </c>
       <c r="B109" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="C109" t="s">
         <v>441</v>
@@ -25871,7 +25883,7 @@
         <v>226</v>
       </c>
       <c r="B110" s="13" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="C110" s="14" t="s">
         <v>442</v>
@@ -25913,7 +25925,7 @@
         <v>226</v>
       </c>
       <c r="B112" s="16" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C112" s="16" t="s">
         <v>443</v>
@@ -25934,7 +25946,7 @@
         <v>226</v>
       </c>
       <c r="B113" s="16" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="C113" s="16" t="s">
         <v>931</v>
@@ -25955,7 +25967,7 @@
         <v>226</v>
       </c>
       <c r="B114" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="C114" t="s">
         <v>506</v>
@@ -26095,7 +26107,7 @@
         <v>226</v>
       </c>
       <c r="B121" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="C121" t="s">
         <v>525</v>
@@ -26281,7 +26293,7 @@
         <v>226</v>
       </c>
       <c r="B130" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="C130" t="s">
         <v>542</v>
@@ -26301,7 +26313,7 @@
         <v>226</v>
       </c>
       <c r="B131" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="C131" t="s">
         <v>543</v>
@@ -26321,7 +26333,7 @@
         <v>226</v>
       </c>
       <c r="B132" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="C132" t="s">
         <v>544</v>
@@ -26341,7 +26353,7 @@
         <v>226</v>
       </c>
       <c r="B133" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="C133" t="s">
         <v>545</v>
@@ -26651,7 +26663,7 @@
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B151" s="2" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.35">
@@ -26671,6 +26683,7 @@
     <sheetView topLeftCell="A46" workbookViewId="0">
       <selection activeCell="B68" sqref="B68"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -26703,7 +26716,7 @@
         <v>168</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>169</v>
@@ -27480,44 +27493,44 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
+        <v>1197</v>
+      </c>
+      <c r="B60" t="s">
+        <v>1205</v>
+      </c>
+      <c r="C60" t="s">
         <v>1198</v>
       </c>
-      <c r="B60" t="s">
-        <v>1206</v>
-      </c>
-      <c r="C60" t="s">
+      <c r="D60" t="s">
         <v>1199</v>
-      </c>
-      <c r="D60" t="s">
-        <v>1200</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
+        <v>1200</v>
+      </c>
+      <c r="B61" t="s">
+        <v>1206</v>
+      </c>
+      <c r="C61" t="s">
         <v>1201</v>
       </c>
-      <c r="B61" t="s">
-        <v>1207</v>
-      </c>
-      <c r="C61" t="s">
-        <v>1202</v>
-      </c>
       <c r="D61" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
+        <v>1202</v>
+      </c>
+      <c r="B62" t="s">
+        <v>1207</v>
+      </c>
+      <c r="C62" t="s">
         <v>1203</v>
       </c>
-      <c r="B62" t="s">
-        <v>1208</v>
-      </c>
-      <c r="C62" t="s">
-        <v>1204</v>
-      </c>
       <c r="D62" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
@@ -27690,13 +27703,13 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="B75" t="s">
         <v>809</v>
       </c>
       <c r="C75" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="D75" t="s">
         <v>736</v>
@@ -27704,13 +27717,13 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="B76" t="s">
         <v>810</v>
       </c>
       <c r="C76" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="D76" t="s">
         <v>736</v>
@@ -27718,13 +27731,13 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="B77" t="s">
         <v>811</v>
       </c>
       <c r="C77" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="D77" t="s">
         <v>736</v>
@@ -28882,11 +28895,12 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:G121"/>
+  <dimension ref="A1:G124"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42:XFD42"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72"/>
     </sheetView>
+    <sheetView topLeftCell="A31" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -29234,7 +29248,7 @@
         <v>916</v>
       </c>
       <c r="B29" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="C29" t="s">
         <v>515</v>
@@ -29251,353 +29265,353 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>1099</v>
+        <v>916</v>
       </c>
       <c r="B30" t="s">
-        <v>1097</v>
+        <v>284</v>
       </c>
       <c r="C30" t="s">
-        <v>217</v>
+        <v>515</v>
       </c>
       <c r="D30" t="s">
-        <v>19</v>
+        <v>285</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>1098</v>
+        <v>423</v>
       </c>
       <c r="F30" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>914</v>
+        <v>405</v>
       </c>
       <c r="B31" t="s">
-        <v>115</v>
+        <v>1097</v>
       </c>
       <c r="C31" t="s">
-        <v>509</v>
+        <v>217</v>
       </c>
       <c r="D31" t="s">
-        <v>142</v>
+        <v>19</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>375</v>
+        <v>1098</v>
       </c>
       <c r="F31" t="s">
-        <v>376</v>
+        <v>223</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B32" t="s">
-        <v>1120</v>
+        <v>282</v>
       </c>
       <c r="C32" t="s">
-        <v>541</v>
+        <v>217</v>
       </c>
       <c r="D32" t="s">
-        <v>142</v>
+        <v>19</v>
       </c>
       <c r="E32" s="9" t="s">
         <v>423</v>
       </c>
       <c r="F32" t="s">
-        <v>188</v>
+        <v>223</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>1154</v>
+        <v>914</v>
       </c>
       <c r="B33" t="s">
-        <v>1145</v>
+        <v>115</v>
       </c>
       <c r="C33" t="s">
-        <v>1162</v>
+        <v>509</v>
       </c>
       <c r="D33" t="s">
         <v>142</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>1153</v>
+        <v>375</v>
       </c>
       <c r="F33" t="s">
-        <v>461</v>
+        <v>376</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>1155</v>
+        <v>407</v>
       </c>
       <c r="B34" t="s">
-        <v>1146</v>
+        <v>1119</v>
       </c>
       <c r="C34" t="s">
-        <v>1163</v>
+        <v>541</v>
       </c>
       <c r="D34" t="s">
-        <v>2</v>
+        <v>142</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>1153</v>
+        <v>423</v>
       </c>
       <c r="F34" t="s">
-        <v>462</v>
+        <v>188</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>1156</v>
+        <v>407</v>
       </c>
       <c r="B35" t="s">
-        <v>1147</v>
+        <v>283</v>
       </c>
       <c r="C35" t="s">
-        <v>1164</v>
+        <v>541</v>
       </c>
       <c r="D35" t="s">
         <v>142</v>
       </c>
       <c r="E35" s="9" t="s">
-        <v>1153</v>
+        <v>423</v>
       </c>
       <c r="F35" t="s">
-        <v>461</v>
+        <v>188</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>1157</v>
+        <v>1153</v>
       </c>
       <c r="B36" t="s">
-        <v>1148</v>
+        <v>1144</v>
       </c>
       <c r="C36" t="s">
-        <v>1165</v>
+        <v>1161</v>
       </c>
       <c r="D36" t="s">
-        <v>2</v>
+        <v>142</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="F36" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>1158</v>
+        <v>1154</v>
       </c>
       <c r="B37" t="s">
-        <v>1149</v>
+        <v>1145</v>
       </c>
       <c r="C37" t="s">
-        <v>1166</v>
+        <v>1162</v>
       </c>
       <c r="D37" t="s">
-        <v>142</v>
+        <v>2</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="F37" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>1159</v>
+        <v>1155</v>
       </c>
       <c r="B38" t="s">
-        <v>1150</v>
+        <v>1146</v>
       </c>
       <c r="C38" t="s">
-        <v>1167</v>
+        <v>1163</v>
       </c>
       <c r="D38" t="s">
-        <v>2</v>
+        <v>142</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="F38" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>1160</v>
+        <v>1156</v>
       </c>
       <c r="B39" t="s">
-        <v>1151</v>
+        <v>1147</v>
       </c>
       <c r="C39" t="s">
-        <v>1168</v>
+        <v>1164</v>
       </c>
       <c r="D39" t="s">
-        <v>142</v>
+        <v>2</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="F39" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>1161</v>
+        <v>1157</v>
       </c>
       <c r="B40" t="s">
+        <v>1148</v>
+      </c>
+      <c r="C40" t="s">
+        <v>1165</v>
+      </c>
+      <c r="D40" t="s">
+        <v>142</v>
+      </c>
+      <c r="E40" s="9" t="s">
         <v>1152</v>
       </c>
-      <c r="C40" t="s">
-        <v>1169</v>
-      </c>
-      <c r="D40" t="s">
-        <v>2</v>
-      </c>
-      <c r="E40" s="9" t="s">
-        <v>1153</v>
-      </c>
       <c r="F40" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>408</v>
+        <v>1158</v>
       </c>
       <c r="B41" t="s">
-        <v>116</v>
+        <v>1149</v>
       </c>
       <c r="C41" t="s">
-        <v>394</v>
+        <v>1166</v>
       </c>
       <c r="D41" t="s">
-        <v>117</v>
+        <v>2</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>375</v>
+        <v>1152</v>
       </c>
       <c r="F41" t="s">
-        <v>376</v>
+        <v>462</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>410</v>
+        <v>1159</v>
       </c>
       <c r="B42" t="s">
-        <v>1118</v>
+        <v>1150</v>
       </c>
       <c r="C42" t="s">
-        <v>415</v>
+        <v>1167</v>
       </c>
       <c r="D42" t="s">
-        <v>200</v>
+        <v>142</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>1098</v>
+        <v>1152</v>
       </c>
       <c r="F42" t="s">
-        <v>215</v>
+        <v>461</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>412</v>
+        <v>1160</v>
       </c>
       <c r="B43" t="s">
-        <v>1106</v>
+        <v>1151</v>
       </c>
       <c r="C43" t="s">
-        <v>417</v>
+        <v>1168</v>
       </c>
       <c r="D43" t="s">
-        <v>200</v>
+        <v>2</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>1098</v>
+        <v>1152</v>
       </c>
       <c r="F43" t="s">
-        <v>215</v>
+        <v>462</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="B44" t="s">
-        <v>1125</v>
+        <v>116</v>
       </c>
       <c r="C44" t="s">
-        <v>421</v>
+        <v>394</v>
       </c>
       <c r="D44" t="s">
-        <v>263</v>
+        <v>117</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>1098</v>
+        <v>375</v>
       </c>
       <c r="F44" t="s">
-        <v>214</v>
+        <v>376</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>433</v>
+        <v>410</v>
       </c>
       <c r="B45" t="s">
-        <v>1122</v>
+        <v>1117</v>
       </c>
       <c r="C45" t="s">
-        <v>431</v>
+        <v>415</v>
       </c>
       <c r="D45" t="s">
-        <v>263</v>
+        <v>200</v>
       </c>
       <c r="E45" s="9" t="s">
         <v>1098</v>
       </c>
       <c r="F45" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B46" t="s">
-        <v>1124</v>
+        <v>1105</v>
       </c>
       <c r="C46" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="D46" t="s">
-        <v>263</v>
+        <v>200</v>
       </c>
       <c r="E46" s="9" t="s">
         <v>1098</v>
       </c>
       <c r="F46" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>434</v>
+        <v>413</v>
       </c>
       <c r="B47" t="s">
-        <v>1103</v>
+        <v>1124</v>
       </c>
       <c r="C47" t="s">
-        <v>432</v>
+        <v>421</v>
       </c>
       <c r="D47" t="s">
         <v>263</v>
@@ -29610,17 +29624,17 @@
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A48" s="18" t="s">
-        <v>933</v>
+      <c r="A48" t="s">
+        <v>433</v>
       </c>
       <c r="B48" t="s">
-        <v>1128</v>
+        <v>1121</v>
       </c>
       <c r="C48" t="s">
-        <v>496</v>
+        <v>431</v>
       </c>
       <c r="D48" t="s">
-        <v>203</v>
+        <v>263</v>
       </c>
       <c r="E48" s="9" t="s">
         <v>1098</v>
@@ -29630,58 +29644,57 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A49" s="13" t="s">
-        <v>929</v>
-      </c>
-      <c r="B49" s="13" t="s">
-        <v>1105</v>
-      </c>
-      <c r="C49" s="14" t="s">
-        <v>447</v>
-      </c>
-      <c r="D49" s="14" t="s">
-        <v>39</v>
+      <c r="A49" t="s">
+        <v>414</v>
+      </c>
+      <c r="B49" t="s">
+        <v>1123</v>
+      </c>
+      <c r="C49" t="s">
+        <v>422</v>
+      </c>
+      <c r="D49" t="s">
+        <v>263</v>
       </c>
       <c r="E49" s="9" t="s">
         <v>1098</v>
       </c>
-      <c r="F49" s="14" t="s">
+      <c r="F49" t="s">
         <v>214</v>
       </c>
-      <c r="G49" s="13"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>445</v>
+        <v>434</v>
       </c>
       <c r="B50" t="s">
-        <v>1119</v>
+        <v>1102</v>
       </c>
       <c r="C50" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="D50" t="s">
-        <v>79</v>
+        <v>263</v>
       </c>
       <c r="E50" s="9" t="s">
         <v>1098</v>
       </c>
       <c r="F50" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
-        <v>444</v>
+      <c r="A51" s="18" t="s">
+        <v>933</v>
       </c>
       <c r="B51" t="s">
-        <v>1113</v>
+        <v>1127</v>
       </c>
       <c r="C51" t="s">
-        <v>438</v>
+        <v>496</v>
       </c>
       <c r="D51" t="s">
-        <v>79</v>
+        <v>203</v>
       </c>
       <c r="E51" s="9" t="s">
         <v>1098</v>
@@ -29691,41 +29704,41 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A52" s="16" t="s">
-        <v>930</v>
-      </c>
-      <c r="B52" s="16" t="s">
+      <c r="A52" s="13" t="s">
+        <v>929</v>
+      </c>
+      <c r="B52" s="13" t="s">
         <v>1104</v>
       </c>
-      <c r="C52" s="16" t="s">
-        <v>932</v>
-      </c>
-      <c r="D52" s="16" t="s">
+      <c r="C52" s="14" t="s">
+        <v>447</v>
+      </c>
+      <c r="D52" s="14" t="s">
         <v>39</v>
       </c>
       <c r="E52" s="9" t="s">
         <v>1098</v>
       </c>
-      <c r="F52" s="16" t="s">
+      <c r="F52" s="14" t="s">
         <v>214</v>
       </c>
-      <c r="G52" s="16"/>
+      <c r="G52" s="13"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>410</v>
+        <v>445</v>
       </c>
       <c r="B53" t="s">
-        <v>279</v>
+        <v>1118</v>
       </c>
       <c r="C53" t="s">
-        <v>415</v>
+        <v>437</v>
       </c>
       <c r="D53" t="s">
-        <v>200</v>
+        <v>79</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>423</v>
+        <v>1098</v>
       </c>
       <c r="F53" t="s">
         <v>215</v>
@@ -29733,93 +29746,94 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>412</v>
+        <v>444</v>
       </c>
       <c r="B54" t="s">
-        <v>266</v>
+        <v>1112</v>
       </c>
       <c r="C54" t="s">
-        <v>417</v>
+        <v>438</v>
       </c>
       <c r="D54" t="s">
-        <v>200</v>
+        <v>79</v>
       </c>
       <c r="E54" s="9" t="s">
-        <v>423</v>
+        <v>1098</v>
       </c>
       <c r="F54" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
-        <v>413</v>
-      </c>
-      <c r="B55" t="s">
-        <v>289</v>
-      </c>
-      <c r="C55" t="s">
-        <v>421</v>
-      </c>
-      <c r="D55" t="s">
-        <v>263</v>
+      <c r="A55" s="16" t="s">
+        <v>930</v>
+      </c>
+      <c r="B55" s="16" t="s">
+        <v>1103</v>
+      </c>
+      <c r="C55" s="16" t="s">
+        <v>932</v>
+      </c>
+      <c r="D55" s="16" t="s">
+        <v>39</v>
       </c>
       <c r="E55" s="9" t="s">
-        <v>423</v>
-      </c>
-      <c r="F55" t="s">
+        <v>1098</v>
+      </c>
+      <c r="F55" s="16" t="s">
         <v>214</v>
       </c>
+      <c r="G55" s="16"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>433</v>
+        <v>410</v>
       </c>
       <c r="B56" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="C56" t="s">
-        <v>431</v>
+        <v>415</v>
       </c>
       <c r="D56" t="s">
-        <v>263</v>
+        <v>200</v>
       </c>
       <c r="E56" s="9" t="s">
         <v>423</v>
       </c>
       <c r="F56" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B57" t="s">
-        <v>288</v>
+        <v>266</v>
       </c>
       <c r="C57" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="D57" t="s">
-        <v>263</v>
+        <v>200</v>
       </c>
       <c r="E57" s="9" t="s">
         <v>423</v>
       </c>
       <c r="F57" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>434</v>
+        <v>413</v>
       </c>
       <c r="B58" t="s">
-        <v>262</v>
+        <v>289</v>
       </c>
       <c r="C58" t="s">
-        <v>432</v>
+        <v>421</v>
       </c>
       <c r="D58" t="s">
         <v>263</v>
@@ -29832,17 +29846,17 @@
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A59" s="18" t="s">
-        <v>933</v>
+      <c r="A59" t="s">
+        <v>433</v>
       </c>
       <c r="B59" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="C59" t="s">
-        <v>496</v>
+        <v>431</v>
       </c>
       <c r="D59" t="s">
-        <v>203</v>
+        <v>263</v>
       </c>
       <c r="E59" s="9" t="s">
         <v>423</v>
@@ -29852,58 +29866,57 @@
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A60" s="13" t="s">
-        <v>929</v>
-      </c>
-      <c r="B60" s="13" t="s">
-        <v>265</v>
-      </c>
-      <c r="C60" s="14" t="s">
-        <v>447</v>
-      </c>
-      <c r="D60" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="E60" s="15" t="s">
-        <v>423</v>
-      </c>
-      <c r="F60" s="14" t="s">
+      <c r="A60" t="s">
+        <v>414</v>
+      </c>
+      <c r="B60" t="s">
+        <v>288</v>
+      </c>
+      <c r="C60" t="s">
+        <v>422</v>
+      </c>
+      <c r="D60" t="s">
+        <v>263</v>
+      </c>
+      <c r="E60" s="9" t="s">
+        <v>423</v>
+      </c>
+      <c r="F60" t="s">
         <v>214</v>
       </c>
-      <c r="G60" s="13"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>445</v>
+        <v>434</v>
       </c>
       <c r="B61" t="s">
-        <v>280</v>
+        <v>262</v>
       </c>
       <c r="C61" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="D61" t="s">
-        <v>79</v>
+        <v>263</v>
       </c>
       <c r="E61" s="9" t="s">
         <v>423</v>
       </c>
       <c r="F61" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
-        <v>444</v>
+      <c r="A62" s="18" t="s">
+        <v>933</v>
       </c>
       <c r="B62" t="s">
-        <v>270</v>
+        <v>292</v>
       </c>
       <c r="C62" t="s">
-        <v>438</v>
+        <v>496</v>
       </c>
       <c r="D62" t="s">
-        <v>79</v>
+        <v>203</v>
       </c>
       <c r="E62" s="9" t="s">
         <v>423</v>
@@ -29913,98 +29926,99 @@
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A63" s="16" t="s">
-        <v>930</v>
-      </c>
-      <c r="B63" s="16" t="s">
-        <v>264</v>
-      </c>
-      <c r="C63" s="16" t="s">
-        <v>932</v>
-      </c>
-      <c r="D63" s="16" t="s">
+      <c r="A63" s="13" t="s">
+        <v>929</v>
+      </c>
+      <c r="B63" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="C63" s="14" t="s">
+        <v>447</v>
+      </c>
+      <c r="D63" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="E63" s="17" t="s">
-        <v>423</v>
-      </c>
-      <c r="F63" s="16" t="s">
+      <c r="E63" s="15" t="s">
+        <v>423</v>
+      </c>
+      <c r="F63" s="14" t="s">
         <v>214</v>
       </c>
-      <c r="G63" s="16"/>
+      <c r="G63" s="13"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>937</v>
+        <v>445</v>
       </c>
       <c r="B64" t="s">
-        <v>244</v>
+        <v>280</v>
       </c>
       <c r="C64" t="s">
-        <v>550</v>
+        <v>437</v>
       </c>
       <c r="D64" t="s">
-        <v>534</v>
+        <v>79</v>
       </c>
       <c r="E64" s="9" t="s">
         <v>423</v>
       </c>
       <c r="F64" t="s">
-        <v>188</v>
+        <v>215</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>923</v>
+        <v>444</v>
       </c>
       <c r="B65" t="s">
-        <v>245</v>
+        <v>270</v>
       </c>
       <c r="C65" t="s">
-        <v>536</v>
+        <v>438</v>
       </c>
       <c r="D65" t="s">
-        <v>534</v>
+        <v>79</v>
       </c>
       <c r="E65" s="9" t="s">
         <v>423</v>
       </c>
       <c r="F65" t="s">
-        <v>188</v>
+        <v>214</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A66" t="s">
-        <v>926</v>
-      </c>
-      <c r="B66" t="s">
-        <v>247</v>
-      </c>
-      <c r="C66" t="s">
-        <v>547</v>
-      </c>
-      <c r="D66" t="s">
-        <v>5</v>
-      </c>
-      <c r="E66" s="9" t="s">
-        <v>423</v>
-      </c>
-      <c r="F66" t="s">
-        <v>188</v>
-      </c>
+      <c r="A66" s="16" t="s">
+        <v>930</v>
+      </c>
+      <c r="B66" s="16" t="s">
+        <v>264</v>
+      </c>
+      <c r="C66" s="16" t="s">
+        <v>932</v>
+      </c>
+      <c r="D66" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="E66" s="17" t="s">
+        <v>423</v>
+      </c>
+      <c r="F66" s="16" t="s">
+        <v>214</v>
+      </c>
+      <c r="G66" s="16"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>927</v>
+        <v>937</v>
       </c>
       <c r="B67" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C67" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="D67" t="s">
-        <v>5</v>
+        <v>534</v>
       </c>
       <c r="E67" s="9" t="s">
         <v>423</v>
@@ -30015,16 +30029,16 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>928</v>
+        <v>923</v>
       </c>
       <c r="B68" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C68" t="s">
-        <v>549</v>
+        <v>536</v>
       </c>
       <c r="D68" t="s">
-        <v>5</v>
+        <v>534</v>
       </c>
       <c r="E68" s="9" t="s">
         <v>423</v>
@@ -30035,56 +30049,56 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>14</v>
+        <v>926</v>
       </c>
       <c r="B69" t="s">
-        <v>1129</v>
+        <v>247</v>
       </c>
       <c r="C69" t="s">
-        <v>429</v>
+        <v>547</v>
       </c>
       <c r="D69" t="s">
-        <v>203</v>
+        <v>5</v>
       </c>
       <c r="E69" s="9" t="s">
-        <v>1098</v>
+        <v>423</v>
       </c>
       <c r="F69" t="s">
-        <v>215</v>
+        <v>188</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>14</v>
+        <v>927</v>
       </c>
       <c r="B70" t="s">
-        <v>293</v>
+        <v>248</v>
       </c>
       <c r="C70" t="s">
-        <v>429</v>
+        <v>548</v>
       </c>
       <c r="D70" t="s">
-        <v>203</v>
+        <v>5</v>
       </c>
       <c r="E70" s="9" t="s">
         <v>423</v>
       </c>
       <c r="F70" t="s">
-        <v>215</v>
+        <v>188</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>10</v>
+        <v>928</v>
       </c>
       <c r="B71" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C71" t="s">
-        <v>430</v>
+        <v>549</v>
       </c>
       <c r="D71" t="s">
-        <v>203</v>
+        <v>5</v>
       </c>
       <c r="E71" s="9" t="s">
         <v>423</v>
@@ -30095,62 +30109,62 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>226</v>
+        <v>14</v>
       </c>
       <c r="B72" t="s">
-        <v>123</v>
+        <v>1128</v>
       </c>
       <c r="C72" t="s">
-        <v>395</v>
+        <v>429</v>
       </c>
       <c r="D72" t="s">
-        <v>396</v>
+        <v>203</v>
       </c>
       <c r="E72" s="9" t="s">
-        <v>375</v>
+        <v>1098</v>
       </c>
       <c r="F72" t="s">
-        <v>376</v>
+        <v>215</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>226</v>
+        <v>14</v>
       </c>
       <c r="B73" t="s">
-        <v>1107</v>
+        <v>293</v>
       </c>
       <c r="C73" t="s">
-        <v>418</v>
+        <v>429</v>
       </c>
       <c r="D73" t="s">
-        <v>263</v>
+        <v>203</v>
       </c>
       <c r="E73" s="9" t="s">
         <v>423</v>
       </c>
       <c r="F73" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>226</v>
+        <v>10</v>
       </c>
       <c r="B74" t="s">
-        <v>1108</v>
+        <v>252</v>
       </c>
       <c r="C74" t="s">
-        <v>419</v>
+        <v>430</v>
       </c>
       <c r="D74" t="s">
-        <v>263</v>
+        <v>203</v>
       </c>
       <c r="E74" s="9" t="s">
         <v>423</v>
       </c>
       <c r="F74" t="s">
-        <v>214</v>
+        <v>188</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.35">
@@ -30158,19 +30172,19 @@
         <v>226</v>
       </c>
       <c r="B75" t="s">
-        <v>1109</v>
+        <v>123</v>
       </c>
       <c r="C75" t="s">
-        <v>420</v>
+        <v>395</v>
       </c>
       <c r="D75" t="s">
-        <v>263</v>
+        <v>396</v>
       </c>
       <c r="E75" s="9" t="s">
-        <v>423</v>
+        <v>375</v>
       </c>
       <c r="F75" t="s">
-        <v>214</v>
+        <v>376</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.35">
@@ -30178,13 +30192,13 @@
         <v>226</v>
       </c>
       <c r="B76" t="s">
-        <v>1110</v>
+        <v>1106</v>
       </c>
       <c r="C76" t="s">
-        <v>439</v>
+        <v>418</v>
       </c>
       <c r="D76" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="E76" s="9" t="s">
         <v>423</v>
@@ -30198,13 +30212,13 @@
         <v>226</v>
       </c>
       <c r="B77" t="s">
-        <v>1111</v>
+        <v>1107</v>
       </c>
       <c r="C77" t="s">
-        <v>440</v>
+        <v>419</v>
       </c>
       <c r="D77" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="E77" s="9" t="s">
         <v>423</v>
@@ -30218,13 +30232,13 @@
         <v>226</v>
       </c>
       <c r="B78" t="s">
-        <v>1112</v>
+        <v>1108</v>
       </c>
       <c r="C78" t="s">
-        <v>441</v>
+        <v>420</v>
       </c>
       <c r="D78" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="E78" s="9" t="s">
         <v>423</v>
@@ -30234,167 +30248,167 @@
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A79" s="13" t="s">
-        <v>226</v>
-      </c>
-      <c r="B79" s="13" t="s">
+      <c r="A79" t="s">
+        <v>226</v>
+      </c>
+      <c r="B79" t="s">
+        <v>1109</v>
+      </c>
+      <c r="C79" t="s">
+        <v>439</v>
+      </c>
+      <c r="D79" t="s">
+        <v>272</v>
+      </c>
+      <c r="E79" s="9" t="s">
+        <v>423</v>
+      </c>
+      <c r="F79" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>226</v>
+      </c>
+      <c r="B80" t="s">
+        <v>1110</v>
+      </c>
+      <c r="C80" t="s">
+        <v>440</v>
+      </c>
+      <c r="D80" t="s">
+        <v>272</v>
+      </c>
+      <c r="E80" s="9" t="s">
+        <v>423</v>
+      </c>
+      <c r="F80" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>226</v>
+      </c>
+      <c r="B81" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C81" t="s">
+        <v>441</v>
+      </c>
+      <c r="D81" t="s">
+        <v>272</v>
+      </c>
+      <c r="E81" s="9" t="s">
+        <v>423</v>
+      </c>
+      <c r="F81" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A82" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="B82" s="13" t="s">
+        <v>1125</v>
+      </c>
+      <c r="C82" s="14" t="s">
+        <v>442</v>
+      </c>
+      <c r="D82" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E82" s="15" t="s">
+        <v>423</v>
+      </c>
+      <c r="F82" s="14" t="s">
+        <v>214</v>
+      </c>
+      <c r="G82" s="14"/>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A83" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="B83" s="14" t="s">
+        <v>227</v>
+      </c>
+      <c r="C83" s="14" t="s">
+        <v>377</v>
+      </c>
+      <c r="D83" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E83" s="15" t="s">
+        <v>423</v>
+      </c>
+      <c r="F83" s="14" t="s">
+        <v>380</v>
+      </c>
+      <c r="G83" s="13"/>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A84" s="16" t="s">
+        <v>226</v>
+      </c>
+      <c r="B84" s="16" t="s">
         <v>1126</v>
       </c>
-      <c r="C79" s="14" t="s">
-        <v>442</v>
-      </c>
-      <c r="D79" s="14" t="s">
+      <c r="C84" s="16" t="s">
+        <v>443</v>
+      </c>
+      <c r="D84" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="E79" s="15" t="s">
-        <v>423</v>
-      </c>
-      <c r="F79" s="14" t="s">
+      <c r="E84" s="17" t="s">
+        <v>423</v>
+      </c>
+      <c r="F84" s="16" t="s">
         <v>214</v>
       </c>
-      <c r="G79" s="14"/>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A80" s="13" t="s">
-        <v>226</v>
-      </c>
-      <c r="B80" s="14" t="s">
-        <v>227</v>
-      </c>
-      <c r="C80" s="14" t="s">
-        <v>377</v>
-      </c>
-      <c r="D80" s="14" t="s">
+      <c r="G84" s="16"/>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A85" s="16" t="s">
+        <v>226</v>
+      </c>
+      <c r="B85" s="16" t="s">
+        <v>1122</v>
+      </c>
+      <c r="C85" s="16" t="s">
+        <v>931</v>
+      </c>
+      <c r="D85" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="E80" s="15" t="s">
-        <v>423</v>
-      </c>
-      <c r="F80" s="14" t="s">
-        <v>380</v>
-      </c>
-      <c r="G80" s="13"/>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A81" s="16" t="s">
-        <v>226</v>
-      </c>
-      <c r="B81" s="16" t="s">
-        <v>1127</v>
-      </c>
-      <c r="C81" s="16" t="s">
-        <v>443</v>
-      </c>
-      <c r="D81" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="E81" s="17" t="s">
-        <v>423</v>
-      </c>
-      <c r="F81" s="16" t="s">
+      <c r="E85" s="17" t="s">
+        <v>423</v>
+      </c>
+      <c r="F85" s="16" t="s">
         <v>214</v>
       </c>
-      <c r="G81" s="16"/>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A82" s="16" t="s">
-        <v>226</v>
-      </c>
-      <c r="B82" s="16" t="s">
-        <v>1123</v>
-      </c>
-      <c r="C82" s="16" t="s">
-        <v>931</v>
-      </c>
-      <c r="D82" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="E82" s="17" t="s">
-        <v>423</v>
-      </c>
-      <c r="F82" s="16" t="s">
-        <v>214</v>
-      </c>
-      <c r="G82" s="16"/>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A83" t="s">
-        <v>226</v>
-      </c>
-      <c r="B83" t="s">
-        <v>1130</v>
-      </c>
-      <c r="C83" t="s">
-        <v>506</v>
-      </c>
-      <c r="D83" t="s">
-        <v>51</v>
-      </c>
-      <c r="E83" s="9" t="s">
-        <v>423</v>
-      </c>
-      <c r="F83" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A84" t="s">
-        <v>226</v>
-      </c>
-      <c r="B84" t="s">
-        <v>255</v>
-      </c>
-      <c r="C84" t="s">
-        <v>508</v>
-      </c>
-      <c r="D84" t="s">
-        <v>51</v>
-      </c>
-      <c r="E84" s="9" t="s">
-        <v>423</v>
-      </c>
-      <c r="F84" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A85" t="s">
-        <v>226</v>
-      </c>
-      <c r="B85" t="s">
-        <v>118</v>
-      </c>
-      <c r="C85" t="s">
-        <v>514</v>
-      </c>
-      <c r="D85" t="s">
-        <v>372</v>
-      </c>
-      <c r="E85" s="9" t="s">
-        <v>375</v>
-      </c>
-      <c r="F85" t="s">
-        <v>376</v>
-      </c>
+      <c r="G85" s="16"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>226</v>
       </c>
       <c r="B86" t="s">
-        <v>120</v>
+        <v>1129</v>
       </c>
       <c r="C86" t="s">
-        <v>513</v>
+        <v>506</v>
       </c>
       <c r="D86" t="s">
-        <v>372</v>
+        <v>51</v>
       </c>
       <c r="E86" s="9" t="s">
-        <v>375</v>
+        <v>423</v>
       </c>
       <c r="F86" t="s">
-        <v>376</v>
+        <v>215</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.35">
@@ -30402,19 +30416,19 @@
         <v>226</v>
       </c>
       <c r="B87" t="s">
-        <v>190</v>
+        <v>255</v>
       </c>
       <c r="C87" t="s">
-        <v>204</v>
+        <v>508</v>
       </c>
       <c r="D87" t="s">
-        <v>203</v>
+        <v>51</v>
       </c>
       <c r="E87" s="9" t="s">
-        <v>375</v>
+        <v>423</v>
       </c>
       <c r="F87" t="s">
-        <v>376</v>
+        <v>188</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.35">
@@ -30422,19 +30436,19 @@
         <v>226</v>
       </c>
       <c r="B88" t="s">
-        <v>361</v>
+        <v>118</v>
       </c>
       <c r="C88" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="D88" t="s">
-        <v>39</v>
+        <v>372</v>
       </c>
       <c r="E88" s="9" t="s">
-        <v>125</v>
+        <v>375</v>
       </c>
       <c r="F88" t="s">
-        <v>522</v>
+        <v>376</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.35">
@@ -30442,19 +30456,19 @@
         <v>226</v>
       </c>
       <c r="B89" t="s">
-        <v>362</v>
+        <v>120</v>
       </c>
       <c r="C89" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
       <c r="D89" t="s">
-        <v>39</v>
+        <v>372</v>
       </c>
       <c r="E89" s="9" t="s">
-        <v>125</v>
+        <v>375</v>
       </c>
       <c r="F89" t="s">
-        <v>522</v>
+        <v>376</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.35">
@@ -30462,19 +30476,19 @@
         <v>226</v>
       </c>
       <c r="B90" t="s">
-        <v>1131</v>
+        <v>190</v>
       </c>
       <c r="C90" t="s">
-        <v>525</v>
+        <v>204</v>
       </c>
       <c r="D90" t="s">
-        <v>51</v>
+        <v>203</v>
       </c>
       <c r="E90" s="9" t="s">
-        <v>1098</v>
+        <v>375</v>
       </c>
       <c r="F90" t="s">
-        <v>449</v>
+        <v>376</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.35">
@@ -30482,19 +30496,19 @@
         <v>226</v>
       </c>
       <c r="B91" t="s">
-        <v>124</v>
+        <v>361</v>
       </c>
       <c r="C91" t="s">
-        <v>527</v>
+        <v>518</v>
       </c>
       <c r="D91" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="E91" s="9" t="s">
-        <v>375</v>
+        <v>125</v>
       </c>
       <c r="F91" t="s">
-        <v>376</v>
+        <v>522</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.35">
@@ -30502,22 +30516,19 @@
         <v>226</v>
       </c>
       <c r="B92" t="s">
-        <v>257</v>
+        <v>362</v>
       </c>
       <c r="C92" t="s">
-        <v>529</v>
+        <v>519</v>
       </c>
       <c r="D92" t="s">
-        <v>203</v>
+        <v>39</v>
       </c>
       <c r="E92" s="9" t="s">
-        <v>423</v>
+        <v>125</v>
       </c>
       <c r="F92" t="s">
-        <v>188</v>
-      </c>
-      <c r="G92" s="2" t="s">
-        <v>646</v>
+        <v>522</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.35">
@@ -30525,22 +30536,19 @@
         <v>226</v>
       </c>
       <c r="B93" t="s">
-        <v>256</v>
+        <v>1130</v>
       </c>
       <c r="C93" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="D93" t="s">
-        <v>203</v>
+        <v>51</v>
       </c>
       <c r="E93" s="9" t="s">
-        <v>423</v>
+        <v>1098</v>
       </c>
       <c r="F93" t="s">
-        <v>188</v>
-      </c>
-      <c r="G93" s="2" t="s">
-        <v>646</v>
+        <v>449</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.35">
@@ -30548,13 +30556,13 @@
         <v>226</v>
       </c>
       <c r="B94" t="s">
-        <v>86</v>
+        <v>124</v>
       </c>
       <c r="C94" t="s">
-        <v>651</v>
+        <v>527</v>
       </c>
       <c r="D94" t="s">
-        <v>534</v>
+        <v>51</v>
       </c>
       <c r="E94" s="9" t="s">
         <v>375</v>
@@ -30568,13 +30576,13 @@
         <v>226</v>
       </c>
       <c r="B95" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C95" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="D95" t="s">
-        <v>253</v>
+        <v>203</v>
       </c>
       <c r="E95" s="9" t="s">
         <v>423</v>
@@ -30582,16 +30590,19 @@
       <c r="F95" t="s">
         <v>188</v>
       </c>
+      <c r="G95" s="2" t="s">
+        <v>646</v>
+      </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>226</v>
       </c>
       <c r="B96" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="C96" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
       <c r="D96" t="s">
         <v>203</v>
@@ -30602,25 +30613,28 @@
       <c r="F96" t="s">
         <v>188</v>
       </c>
+      <c r="G96" s="2" t="s">
+        <v>646</v>
+      </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>226</v>
       </c>
       <c r="B97" t="s">
-        <v>258</v>
+        <v>86</v>
       </c>
       <c r="C97" t="s">
-        <v>535</v>
+        <v>651</v>
       </c>
       <c r="D97" t="s">
-        <v>203</v>
+        <v>534</v>
       </c>
       <c r="E97" s="9" t="s">
-        <v>423</v>
+        <v>375</v>
       </c>
       <c r="F97" t="s">
-        <v>188</v>
+        <v>376</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.35">
@@ -30628,19 +30642,19 @@
         <v>226</v>
       </c>
       <c r="B98" t="s">
-        <v>228</v>
+        <v>259</v>
       </c>
       <c r="C98" t="s">
-        <v>378</v>
+        <v>532</v>
       </c>
       <c r="D98" t="s">
-        <v>229</v>
+        <v>253</v>
       </c>
       <c r="E98" s="9" t="s">
         <v>423</v>
       </c>
       <c r="F98" t="s">
-        <v>380</v>
+        <v>188</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.35">
@@ -30648,13 +30662,13 @@
         <v>226</v>
       </c>
       <c r="B99" t="s">
-        <v>1114</v>
+        <v>251</v>
       </c>
       <c r="C99" t="s">
-        <v>542</v>
+        <v>533</v>
       </c>
       <c r="D99" t="s">
-        <v>142</v>
+        <v>203</v>
       </c>
       <c r="E99" s="9" t="s">
         <v>423</v>
@@ -30668,13 +30682,13 @@
         <v>226</v>
       </c>
       <c r="B100" t="s">
-        <v>1115</v>
+        <v>258</v>
       </c>
       <c r="C100" t="s">
-        <v>543</v>
+        <v>535</v>
       </c>
       <c r="D100" t="s">
-        <v>385</v>
+        <v>203</v>
       </c>
       <c r="E100" s="9" t="s">
         <v>423</v>
@@ -30688,19 +30702,19 @@
         <v>226</v>
       </c>
       <c r="B101" t="s">
-        <v>1116</v>
+        <v>228</v>
       </c>
       <c r="C101" t="s">
-        <v>544</v>
+        <v>378</v>
       </c>
       <c r="D101" t="s">
-        <v>385</v>
+        <v>229</v>
       </c>
       <c r="E101" s="9" t="s">
         <v>423</v>
       </c>
       <c r="F101" t="s">
-        <v>188</v>
+        <v>380</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.35">
@@ -30708,13 +30722,13 @@
         <v>226</v>
       </c>
       <c r="B102" t="s">
-        <v>1117</v>
+        <v>1113</v>
       </c>
       <c r="C102" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="D102" t="s">
-        <v>385</v>
+        <v>142</v>
       </c>
       <c r="E102" s="9" t="s">
         <v>423</v>
@@ -30728,13 +30742,13 @@
         <v>226</v>
       </c>
       <c r="B103" t="s">
-        <v>250</v>
+        <v>1114</v>
       </c>
       <c r="C103" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="D103" t="s">
-        <v>142</v>
+        <v>385</v>
       </c>
       <c r="E103" s="9" t="s">
         <v>423</v>
@@ -30748,19 +30762,19 @@
         <v>226</v>
       </c>
       <c r="B104" t="s">
-        <v>231</v>
+        <v>1115</v>
       </c>
       <c r="C104" t="s">
-        <v>381</v>
+        <v>544</v>
       </c>
       <c r="D104" t="s">
-        <v>142</v>
+        <v>385</v>
       </c>
       <c r="E104" s="9" t="s">
         <v>423</v>
       </c>
       <c r="F104" t="s">
-        <v>380</v>
+        <v>188</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.35">
@@ -30768,10 +30782,10 @@
         <v>226</v>
       </c>
       <c r="B105" t="s">
-        <v>232</v>
+        <v>1116</v>
       </c>
       <c r="C105" t="s">
-        <v>382</v>
+        <v>545</v>
       </c>
       <c r="D105" t="s">
         <v>385</v>
@@ -30780,7 +30794,7 @@
         <v>423</v>
       </c>
       <c r="F105" t="s">
-        <v>380</v>
+        <v>188</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.35">
@@ -30788,19 +30802,19 @@
         <v>226</v>
       </c>
       <c r="B106" t="s">
-        <v>233</v>
+        <v>250</v>
       </c>
       <c r="C106" t="s">
-        <v>383</v>
+        <v>546</v>
       </c>
       <c r="D106" t="s">
-        <v>385</v>
+        <v>142</v>
       </c>
       <c r="E106" s="9" t="s">
         <v>423</v>
       </c>
       <c r="F106" t="s">
-        <v>380</v>
+        <v>188</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.35">
@@ -30808,13 +30822,13 @@
         <v>226</v>
       </c>
       <c r="B107" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C107" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="D107" t="s">
-        <v>385</v>
+        <v>142</v>
       </c>
       <c r="E107" s="9" t="s">
         <v>423</v>
@@ -30828,13 +30842,13 @@
         <v>226</v>
       </c>
       <c r="B108" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C108" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="D108" t="s">
-        <v>5</v>
+        <v>385</v>
       </c>
       <c r="E108" s="9" t="s">
         <v>423</v>
@@ -30848,19 +30862,19 @@
         <v>226</v>
       </c>
       <c r="B109" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C109" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="D109" t="s">
-        <v>5</v>
+        <v>385</v>
       </c>
       <c r="E109" s="9" t="s">
         <v>423</v>
       </c>
       <c r="F109" t="s">
-        <v>188</v>
+        <v>380</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.35">
@@ -30868,19 +30882,19 @@
         <v>226</v>
       </c>
       <c r="B110" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C110" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="D110" t="s">
-        <v>237</v>
+        <v>385</v>
       </c>
       <c r="E110" s="9" t="s">
         <v>423</v>
       </c>
       <c r="F110" t="s">
-        <v>188</v>
+        <v>380</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.35">
@@ -30888,19 +30902,19 @@
         <v>226</v>
       </c>
       <c r="B111" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="C111" t="s">
-        <v>390</v>
+        <v>379</v>
       </c>
       <c r="D111" t="s">
-        <v>237</v>
+        <v>5</v>
       </c>
       <c r="E111" s="9" t="s">
         <v>423</v>
       </c>
       <c r="F111" t="s">
-        <v>188</v>
+        <v>380</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.35">
@@ -30908,10 +30922,10 @@
         <v>226</v>
       </c>
       <c r="B112" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C112" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D112" t="s">
         <v>5</v>
@@ -30928,10 +30942,10 @@
         <v>226</v>
       </c>
       <c r="B113" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C113" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D113" t="s">
         <v>237</v>
@@ -30948,13 +30962,13 @@
         <v>226</v>
       </c>
       <c r="B114" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C114" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="D114" t="s">
-        <v>5</v>
+        <v>237</v>
       </c>
       <c r="E114" s="9" t="s">
         <v>423</v>
@@ -30968,13 +30982,13 @@
         <v>226</v>
       </c>
       <c r="B115" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="C115" t="s">
-        <v>936</v>
+        <v>387</v>
       </c>
       <c r="D115" t="s">
-        <v>534</v>
+        <v>5</v>
       </c>
       <c r="E115" s="9" t="s">
         <v>423</v>
@@ -30982,47 +30996,107 @@
       <c r="F115" t="s">
         <v>188</v>
       </c>
-      <c r="G115" t="s">
-        <v>553</v>
-      </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>226</v>
       </c>
       <c r="B116" t="s">
+        <v>240</v>
+      </c>
+      <c r="C116" t="s">
+        <v>391</v>
+      </c>
+      <c r="D116" t="s">
+        <v>237</v>
+      </c>
+      <c r="E116" s="9" t="s">
+        <v>423</v>
+      </c>
+      <c r="F116" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
+        <v>226</v>
+      </c>
+      <c r="B117" t="s">
+        <v>241</v>
+      </c>
+      <c r="C117" t="s">
+        <v>388</v>
+      </c>
+      <c r="D117" t="s">
+        <v>5</v>
+      </c>
+      <c r="E117" s="9" t="s">
+        <v>423</v>
+      </c>
+      <c r="F117" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
+        <v>226</v>
+      </c>
+      <c r="B118" t="s">
+        <v>246</v>
+      </c>
+      <c r="C118" t="s">
+        <v>936</v>
+      </c>
+      <c r="D118" t="s">
+        <v>534</v>
+      </c>
+      <c r="E118" s="9" t="s">
+        <v>423</v>
+      </c>
+      <c r="F118" t="s">
+        <v>188</v>
+      </c>
+      <c r="G118" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
+        <v>226</v>
+      </c>
+      <c r="B119" t="s">
         <v>242</v>
       </c>
-      <c r="C116" s="2"/>
-      <c r="D116" t="s">
+      <c r="C119" s="2"/>
+      <c r="D119" t="s">
         <v>5</v>
       </c>
-      <c r="G116" s="2" t="s">
+      <c r="G119" s="2" t="s">
         <v>1079</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B117" s="2" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B118" s="2" t="s">
-        <v>1096</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B119" s="2" t="s">
-        <v>1095</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B120" s="2" t="s">
-        <v>1113</v>
+        <v>243</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B121" s="2" t="s">
+        <v>1096</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B122" s="2" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B123" s="2" t="s">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B124" s="2" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Bernard lake configuration
</commit_message>
<xml_diff>
--- a/Resources/Variable_description_full.xlsx
+++ b/Resources/Variable_description_full.xlsx
@@ -1,12 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="177" documentId="13_ncr:1_{D9D14E5E-F476-45BE-9422-600D3D140919}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB58738D-6CB9-47F4-9630-7C76AF50602B}"/>
+  <xr:revisionPtr revIDLastSave="182" documentId="13_ncr:1_{D9D14E5E-F476-45BE-9422-600D3D140919}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9E006AD-A564-4CB4-BA64-270727455EBA}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15720" tabRatio="819" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15720" tabRatio="827" activeTab="9" xr2:uid="{FA0D2C8C-B83F-42B3-AEE0-8A421FCD5665}"/>
+    <workbookView minimized="1" xWindow="-21345" yWindow="4560" windowWidth="14400" windowHeight="7275" tabRatio="827" firstSheet="1" activeTab="11" xr2:uid="{FA0D2C8C-B83F-42B3-AEE0-8A421FCD5665}"/>
   </bookViews>
   <sheets>
     <sheet name="Berge_cs" sheetId="1" r:id="rId1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7907" uniqueCount="1226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7912" uniqueCount="1231">
   <si>
     <t>LI-7700</t>
   </si>
@@ -3712,6 +3711,21 @@
   </si>
   <si>
     <t>61205V</t>
+  </si>
+  <si>
+    <t>lux</t>
+  </si>
+  <si>
+    <t>MX2202 Pendant</t>
+  </si>
+  <si>
+    <t>Temperature/light sensor - Datalogger</t>
+  </si>
+  <si>
+    <t>Intensity</t>
+  </si>
+  <si>
+    <t>Light intensity</t>
   </si>
 </sst>
 </file>
@@ -4139,10 +4153,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G180"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58"/>
-    </sheetView>
-    <sheetView workbookViewId="1">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10:XFD25"/>
     </sheetView>
   </sheetViews>
@@ -7563,10 +7574,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G310"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67"/>
-    </sheetView>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="1"/>
+    <sheetView topLeftCell="A35" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -10047,7 +10055,6 @@
   <dimension ref="A1:E158"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -12107,10 +12114,11 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -12224,6 +12232,23 @@
         <v>665</v>
       </c>
     </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>1229</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1230</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1226</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1227</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1228</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12233,8 +12258,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0"/>
-    <sheetView topLeftCell="A2" workbookViewId="1"/>
+    <sheetView topLeftCell="A2" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -12933,7 +12957,6 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -13000,10 +13023,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E186"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A58" sqref="A58"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -15427,10 +15447,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A09E5EF-45A3-45FC-9489-706089B0F397}">
   <dimension ref="A1:G181"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD25"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -18862,10 +18879,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C4518C3-7192-4DD7-93DF-A109DE8BC3C1}">
   <dimension ref="A1:E186"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -21289,10 +21303,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
-    </sheetView>
-    <sheetView workbookViewId="1">
+    <sheetView workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
@@ -23834,10 +23845,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E158"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -25902,10 +25910,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G168"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD38"/>
-    </sheetView>
-    <sheetView topLeftCell="A5" workbookViewId="1">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -29014,10 +29019,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E168"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -31231,10 +31233,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>